<commit_message>
Finished, with some bugs
</commit_message>
<xml_diff>
--- a/Nationsmöte TEST (Svar) (2).xlsx
+++ b/Nationsmöte TEST (Svar) (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Dokument\voting-vg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1083793-A93F-46FF-AA1C-2D1870541A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E083E2-BC04-4924-A046-EAA82E52709B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,7 +329,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>